<commit_message>
Working on additional analysis. Not yet finalized.
</commit_message>
<xml_diff>
--- a/WS_Prime.xlsx
+++ b/WS_Prime.xlsx
@@ -8757,7 +8757,7 @@
         <v>26</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="D23">
         <v>1989</v>
@@ -11177,7 +11177,7 @@
         <v>147</v>
       </c>
       <c r="C144">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="D144">
         <v>1991</v>
@@ -11637,7 +11637,7 @@
         <v>170</v>
       </c>
       <c r="C167">
-        <v>19.8</v>
+        <v>24.5</v>
       </c>
       <c r="D167">
         <v>1992</v>
@@ -12777,7 +12777,7 @@
         <v>227</v>
       </c>
       <c r="C224">
-        <v>0</v>
+        <v>-1.2</v>
       </c>
       <c r="D224">
         <v>1993</v>
@@ -12837,7 +12837,7 @@
         <v>230</v>
       </c>
       <c r="C227">
-        <v>0</v>
+        <v>24.6</v>
       </c>
       <c r="D227">
         <v>1993</v>
@@ -15977,7 +15977,7 @@
         <v>386</v>
       </c>
       <c r="C384">
-        <v>0</v>
+        <v>52.2</v>
       </c>
       <c r="D384">
         <v>1996</v>
@@ -16357,7 +16357,7 @@
         <v>405</v>
       </c>
       <c r="C403">
-        <v>0</v>
+        <v>40.6</v>
       </c>
       <c r="D403">
         <v>1996</v>
@@ -17577,7 +17577,7 @@
         <v>466</v>
       </c>
       <c r="C464">
-        <v>0</v>
+        <v>20.6</v>
       </c>
       <c r="D464">
         <v>1997</v>
@@ -18417,7 +18417,7 @@
         <v>508</v>
       </c>
       <c r="C506">
-        <v>0</v>
+        <v>21.5</v>
       </c>
       <c r="D506">
         <v>1998</v>
@@ -22037,7 +22037,7 @@
         <v>689</v>
       </c>
       <c r="C687">
-        <v>0</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="D687">
         <v>2001</v>
@@ -23257,7 +23257,7 @@
         <v>750</v>
       </c>
       <c r="C748">
-        <v>0</v>
+        <v>-0.4</v>
       </c>
       <c r="D748">
         <v>2002</v>
@@ -25137,7 +25137,7 @@
         <v>844</v>
       </c>
       <c r="C842">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="D842">
         <v>2003</v>
@@ -25357,7 +25357,7 @@
         <v>855</v>
       </c>
       <c r="C853">
-        <v>0</v>
+        <v>41.3</v>
       </c>
       <c r="D853">
         <v>2004</v>
@@ -25457,7 +25457,7 @@
         <v>860</v>
       </c>
       <c r="C858">
-        <v>0</v>
+        <v>21.3</v>
       </c>
       <c r="D858">
         <v>2004</v>
@@ -25917,7 +25917,7 @@
         <v>883</v>
       </c>
       <c r="C881">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="D881">
         <v>2004</v>
@@ -26797,7 +26797,7 @@
         <v>927</v>
       </c>
       <c r="C925">
-        <v>0</v>
+        <v>23.1</v>
       </c>
       <c r="D925">
         <v>2005</v>
@@ -27077,7 +27077,7 @@
         <v>941</v>
       </c>
       <c r="C939">
-        <v>0</v>
+        <v>27.4</v>
       </c>
       <c r="D939">
         <v>2005</v>
@@ -27217,7 +27217,7 @@
         <v>948</v>
       </c>
       <c r="C946">
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="D946">
         <v>2005</v>
@@ -30437,7 +30437,7 @@
         <v>1106</v>
       </c>
       <c r="C1107">
-        <v>0</v>
+        <v>38.9</v>
       </c>
       <c r="D1107">
         <v>2008</v>
@@ -30997,7 +30997,7 @@
         <v>1134</v>
       </c>
       <c r="C1135">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="D1135">
         <v>2008</v>
@@ -32317,7 +32317,7 @@
         <v>1200</v>
       </c>
       <c r="C1201">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D1201">
         <v>2009</v>
@@ -33577,7 +33577,7 @@
         <v>1263</v>
       </c>
       <c r="C1264">
-        <v>0</v>
+        <v>44.7</v>
       </c>
       <c r="D1264">
         <v>2011</v>

</xml_diff>